<commit_message>
code for changes in financial variables
</commit_message>
<xml_diff>
--- a/Variable Index.xlsx
+++ b/Variable Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\Stat-222-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FD74BF-EBB6-4DC6-8A5C-86AE3603D08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0D87F2-EF59-43E3-96C9-C3675FC4A526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1426,11 +1426,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H160"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,9 +1443,10 @@
     <col min="6" max="6" width="26.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1470,8 +1471,9 @@
       <c r="H1" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>134</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>127</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>128</v>
       </c>
@@ -1548,7 +1550,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>129</v>
       </c>
@@ -1568,7 +1570,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>130</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>131</v>
       </c>
@@ -1608,7 +1610,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>132</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>133</v>
       </c>
@@ -1648,7 +1650,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>147</v>
       </c>
@@ -1665,7 +1667,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>148</v>
       </c>
@@ -1682,7 +1684,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>149</v>
       </c>
@@ -1699,7 +1701,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>150</v>
       </c>
@@ -1716,7 +1718,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>151</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
remove date variables from models
</commit_message>
<xml_diff>
--- a/Variable Index.xlsx
+++ b/Variable Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\Stat-222-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7B6BB1-8478-417B-AEB5-D2D81A91564C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D02943-62C5-4371-8570-AC0ED845B431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$173</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="380">
   <si>
     <t>column_name</t>
   </si>
@@ -1532,7 +1532,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F10" sqref="F10"/>
+      <selection pane="topRight" activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2224,18 +2224,7 @@
       <c r="D32" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>341</v>
-      </c>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -3394,18 +3383,7 @@
       <c r="D77" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>341</v>
-      </c>
+      <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
@@ -4200,18 +4178,7 @@
       <c r="D108" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H108" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K108" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>341</v>
-      </c>
+      <c r="I108" s="2"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
@@ -4969,18 +4936,7 @@
       <c r="D137" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H137" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I137" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K137" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="L137" s="2" t="s">
-        <v>341</v>
-      </c>
+      <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
@@ -4995,18 +4951,7 @@
       <c r="D138" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="H138" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I138" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="K138" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="L138" s="2" t="s">
-        <v>341</v>
-      </c>
+      <c r="I138" s="2"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
@@ -5727,7 +5672,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:F173" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F161">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>

<commit_message>
add sector to change model
</commit_message>
<xml_diff>
--- a/Variable Index.xlsx
+++ b/Variable Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\Stat-222-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC14A0-F123-4385-BD76-B7E9875E40C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46611860-D6F9-4E0A-9B3F-2BCB93E57054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="449">
   <si>
     <t>column_name</t>
   </si>
@@ -1737,9 +1737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5571,6 +5571,12 @@
       <c r="I159" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="K159" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="L159" s="2" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">

</xml_diff>